<commit_message>
[ATW] House Decor 수정 $
</commit_message>
<xml_diff>
--- a/Data/[ATW] House Decor - 2907376077/2907376077.xlsx
+++ b/Data/[ATW] House Decor - 2907376077/2907376077.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.7.3\[ATW] House Decor - 2907376077\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\[ATW] House Decor - 2907376077\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682412E6-D7AF-4D05-8915-45B8BB10D3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC058CDC-AE49-4D1A-90C5-343AAC97CC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -270,19 +270,10 @@
     <t>A simple aquarium. Comes with its own locally sourced gravel and tank decorations for its resident goldfish.</t>
   </si>
   <si>
-    <t>designationCategoryDef+Decor.label</t>
-  </si>
-  <si>
-    <t>designationCategoryDef</t>
-  </si>
-  <si>
     <t>Decor.label</t>
   </si>
   <si>
     <t>Decor</t>
-  </si>
-  <si>
-    <t>designationCategoryDef+Decor.description</t>
   </si>
   <si>
     <t>Decor.description</t>
@@ -382,6 +373,18 @@
   </si>
   <si>
     <t>수조에서 물고기를 보는 중</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DesignationCategoryDef+Decor.label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DesignationCategoryDef+Decor.description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DesignationCategoryDef</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -737,7 +740,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -785,7 +788,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -802,7 +805,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -819,7 +822,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -836,7 +839,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -853,7 +856,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -870,7 +873,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -887,7 +890,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -904,7 +907,7 @@
         <v>29</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -921,7 +924,7 @@
         <v>32</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -938,7 +941,7 @@
         <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -955,7 +958,7 @@
         <v>38</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -972,7 +975,7 @@
         <v>41</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -989,7 +992,7 @@
         <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -1006,7 +1009,7 @@
         <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -1023,7 +1026,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -1040,7 +1043,7 @@
         <v>53</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -1057,7 +1060,7 @@
         <v>56</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -1074,7 +1077,7 @@
         <v>59</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -1091,7 +1094,7 @@
         <v>62</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -1108,7 +1111,7 @@
         <v>59</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -1125,7 +1128,7 @@
         <v>67</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -1142,7 +1145,7 @@
         <v>70</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -1159,7 +1162,7 @@
         <v>73</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -1176,58 +1179,58 @@
         <v>76</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>